<commit_message>
login account, fixed bug
</commit_message>
<xml_diff>
--- a/Tracker_Product.xlsx
+++ b/Tracker_Product.xlsx
@@ -84,7 +84,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
@@ -109,9 +109,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
@@ -311,7 +308,7 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Result" displayName="Result" ref="H1:L3" headerRowCount="1" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="H1:L2"/>
+  <autoFilter ref="H1:L3"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Time" dataDxfId="12"/>
     <tableColumn id="2" name="title" dataDxfId="11"/>
@@ -637,7 +634,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -646,7 +643,7 @@
     <col width="21.42578125" customWidth="1" style="1" min="2" max="2"/>
     <col width="15.140625" customWidth="1" style="1" min="3" max="3"/>
     <col width="13" customWidth="1" style="1" min="4" max="4"/>
-    <col width="14.140625" customWidth="1" style="12" min="5" max="5"/>
+    <col width="14.140625" customWidth="1" style="11" min="5" max="5"/>
     <col width="9.140625" customWidth="1" style="1" min="6" max="6"/>
     <col width="9.140625" customWidth="1" style="3" min="7" max="7"/>
     <col width="19.5703125" customWidth="1" style="1" min="8" max="8"/>
@@ -677,7 +674,7 @@
           <t>item/order</t>
         </is>
       </c>
-      <c r="E1" s="12" t="inlineStr">
+      <c r="E1" s="11" t="inlineStr">
         <is>
           <t>price target</t>
         </is>
@@ -728,17 +725,17 @@
       <c r="D2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="12" t="n">
+      <c r="E2" s="11" t="n">
         <v>1000</v>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>pass</t>
+          <t>fail</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>25-May-2021 12h30m</t>
+          <t>25-May-2021 17h01m</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -752,11 +749,11 @@
         </is>
       </c>
       <c r="K2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>pass</t>
+          <t>fail</t>
         </is>
       </c>
     </row>
@@ -768,12 +765,12 @@
         </is>
       </c>
       <c r="C3" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E3" s="12" t="n">
+      <c r="E3" s="11" t="n">
         <v>1000</v>
       </c>
       <c r="F3" t="inlineStr">
@@ -783,7 +780,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>25-May-2021 12h37m</t>
+          <t>25-May-2021 17h07m</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -797,7 +794,7 @@
         </is>
       </c>
       <c r="K3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
@@ -823,7 +820,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -983,7 +980,7 @@
       </c>
       <c r="E7" s="8" t="inlineStr">
         <is>
-          <t>qqqq</t>
+          <t>qyqqyq123</t>
         </is>
       </c>
     </row>

</xml_diff>